<commit_message>
SDGS-19 added span tag to SDG agended references within text
</commit_message>
<xml_diff>
--- a/postprocess/goal_target_list.xlsx
+++ b/postprocess/goal_target_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_JRC\Mapping_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c0ac04fbadbefb8/SDG/Policy-Mapping/postprocess/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23DA0A6-003E-40D1-91FD-24F348D311D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{B23DA0A6-003E-40D1-91FD-24F348D311D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8E684775-4CA8-49D5-BC63-B06F8ED30386}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1586,18 +1586,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1"/>
-    <col min="5" max="5" width="103.44140625" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>73</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>75</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>76</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>77</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>78</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>80</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>81</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>83</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>84</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>85</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>86</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>87</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>88</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>89</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>91</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>92</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>94</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>95</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>96</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>97</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>98</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>99</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>100</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>101</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>102</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>103</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>13</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>14</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>15</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>104</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>105</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>106</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>107</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>108</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>109</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>16</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>110</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>111</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>112</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>18</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>19</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>113</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>114</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>115</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>116</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>117</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>118</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>119</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>120</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>121</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>45</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>20</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>21</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>122</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>123</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>124</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>125</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>126</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>22</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>23</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>24</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>127</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>128</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>129</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>130</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>131</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>132</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>133</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>25</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>26</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>27</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>134</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>135</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>136</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>137</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>138</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>139</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>140</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>28</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>29</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>30</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>141</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>142</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>143</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>144</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>145</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>146</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>147</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>148</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>31</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>32</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>33</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>149</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>150</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>151</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>34</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>35</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>152</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>153</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>154</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>155</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>156</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>157</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>158</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>36</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>37</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>38</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>159</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>160</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>161</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>162</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>163</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>164</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>165</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>166</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>167</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>39</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>40</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>41</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>168</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>169</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>170</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>171</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>172</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>173</v>
       </c>
@@ -4932,7 +4932,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>174</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>175</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>176</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>46</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>42</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>43</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>177</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>178</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>179</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>180</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>181</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>182</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>183</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>184</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>185</v>
       </c>
@@ -5277,7 +5277,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>47</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>186</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>187</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>65</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>66</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>67</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>68</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>69</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>70</v>
       </c>
@@ -5484,7 +5484,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
implemented mapping and plot export of political priorities
</commit_message>
<xml_diff>
--- a/postprocess/goal_target_list.xlsx
+++ b/postprocess/goal_target_list.xlsx
@@ -1,20 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\SDG\Policy-Mapping\postprocess\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4560E4D1-3234-4F61-89F8-9C9ED8FBCF02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="405">
   <si>
     <t>Target</t>
   </si>
@@ -1219,12 +1236,6 @@
     <t>Green Deal</t>
   </si>
   <si>
-    <t>Partnership</t>
-  </si>
-  <si>
-    <t>Digital</t>
-  </si>
-  <si>
     <t>Governance</t>
   </si>
   <si>
@@ -1232,13 +1243,16 @@
   </si>
   <si>
     <t>Migration</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1255,12 +1269,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1290,17 +1310,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1347,7 +1376,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1379,9 +1408,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1413,6 +1460,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1588,14 +1653,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:L170"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +1694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1650,13 +1720,13 @@
         <v>381</v>
       </c>
       <c r="I2" t="s">
+        <v>404</v>
+      </c>
+      <c r="J2" t="s">
         <v>398</v>
       </c>
-      <c r="J2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1682,13 +1752,13 @@
         <v>381</v>
       </c>
       <c r="I3" t="s">
+        <v>404</v>
+      </c>
+      <c r="J3" t="s">
         <v>398</v>
       </c>
-      <c r="J3" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1717,10 +1787,10 @@
         <v>398</v>
       </c>
       <c r="J4" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1746,13 +1816,13 @@
         <v>381</v>
       </c>
       <c r="I5" t="s">
+        <v>404</v>
+      </c>
+      <c r="J5" t="s">
         <v>398</v>
       </c>
-      <c r="J5" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1778,13 +1848,13 @@
         <v>381</v>
       </c>
       <c r="I6" t="s">
+        <v>404</v>
+      </c>
+      <c r="J6" t="s">
         <v>398</v>
       </c>
-      <c r="J6" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1810,13 +1880,13 @@
         <v>381</v>
       </c>
       <c r="I7" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="J7" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1842,13 +1912,13 @@
         <v>381</v>
       </c>
       <c r="I8" t="s">
+        <v>404</v>
+      </c>
+      <c r="J8" t="s">
         <v>398</v>
       </c>
-      <c r="J8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1877,10 +1947,10 @@
         <v>398</v>
       </c>
       <c r="J9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1912,7 +1982,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1941,10 +2011,10 @@
         <v>399</v>
       </c>
       <c r="J11" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1973,10 +2043,10 @@
         <v>400</v>
       </c>
       <c r="J12" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2008,7 +2078,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2037,10 +2107,10 @@
         <v>399</v>
       </c>
       <c r="J14" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2066,13 +2136,13 @@
         <v>382</v>
       </c>
       <c r="I15" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="J15" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2101,10 +2171,10 @@
         <v>399</v>
       </c>
       <c r="J16" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2133,10 +2203,10 @@
         <v>398</v>
       </c>
       <c r="J17" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2165,10 +2235,10 @@
         <v>398</v>
       </c>
       <c r="J18" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2200,7 +2270,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2226,13 +2296,13 @@
         <v>383</v>
       </c>
       <c r="I20" t="s">
+        <v>404</v>
+      </c>
+      <c r="J20" t="s">
         <v>398</v>
       </c>
-      <c r="J20" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2258,13 +2328,13 @@
         <v>383</v>
       </c>
       <c r="I21" t="s">
+        <v>404</v>
+      </c>
+      <c r="J21" t="s">
         <v>398</v>
       </c>
-      <c r="J21" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2290,13 +2360,13 @@
         <v>383</v>
       </c>
       <c r="I22" t="s">
+        <v>404</v>
+      </c>
+      <c r="J22" t="s">
         <v>398</v>
       </c>
-      <c r="J22" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2325,10 +2395,10 @@
         <v>398</v>
       </c>
       <c r="J23" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2357,10 +2427,10 @@
         <v>398</v>
       </c>
       <c r="J24" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2389,10 +2459,10 @@
         <v>400</v>
       </c>
       <c r="J25" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2418,13 +2488,13 @@
         <v>383</v>
       </c>
       <c r="I26" t="s">
+        <v>404</v>
+      </c>
+      <c r="J26" t="s">
         <v>398</v>
       </c>
-      <c r="J26" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2453,10 +2523,10 @@
         <v>398</v>
       </c>
       <c r="J27" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2485,10 +2555,10 @@
         <v>398</v>
       </c>
       <c r="J28" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2517,10 +2587,10 @@
         <v>398</v>
       </c>
       <c r="J29" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2549,10 +2619,10 @@
         <v>398</v>
       </c>
       <c r="J30" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2581,10 +2651,10 @@
         <v>398</v>
       </c>
       <c r="J31" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2610,13 +2680,13 @@
         <v>384</v>
       </c>
       <c r="I32" t="s">
+        <v>404</v>
+      </c>
+      <c r="J32" t="s">
         <v>398</v>
       </c>
-      <c r="J32" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2645,10 +2715,10 @@
         <v>398</v>
       </c>
       <c r="J33" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2677,10 +2747,10 @@
         <v>398</v>
       </c>
       <c r="J34" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2712,7 +2782,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2738,13 +2808,13 @@
         <v>384</v>
       </c>
       <c r="I36" t="s">
+        <v>404</v>
+      </c>
+      <c r="J36" t="s">
         <v>398</v>
       </c>
-      <c r="J36" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2773,10 +2843,10 @@
         <v>398</v>
       </c>
       <c r="J37" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2802,13 +2872,13 @@
         <v>384</v>
       </c>
       <c r="I38" t="s">
+        <v>402</v>
+      </c>
+      <c r="J38" t="s">
         <v>398</v>
       </c>
-      <c r="J38" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2840,7 +2910,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2866,13 +2936,13 @@
         <v>385</v>
       </c>
       <c r="I40" t="s">
+        <v>401</v>
+      </c>
+      <c r="J40" t="s">
         <v>398</v>
       </c>
-      <c r="J40" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2898,13 +2968,13 @@
         <v>385</v>
       </c>
       <c r="I41" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="J41" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2930,13 +3000,13 @@
         <v>385</v>
       </c>
       <c r="I42" t="s">
+        <v>401</v>
+      </c>
+      <c r="J42" t="s">
         <v>398</v>
       </c>
-      <c r="J42" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2962,13 +3032,13 @@
         <v>385</v>
       </c>
       <c r="I43" t="s">
+        <v>404</v>
+      </c>
+      <c r="J43" t="s">
         <v>398</v>
       </c>
-      <c r="J43" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2994,13 +3064,13 @@
         <v>385</v>
       </c>
       <c r="I44" t="s">
+        <v>401</v>
+      </c>
+      <c r="J44" t="s">
         <v>398</v>
       </c>
-      <c r="J44" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3026,13 +3096,13 @@
         <v>385</v>
       </c>
       <c r="I45" t="s">
+        <v>404</v>
+      </c>
+      <c r="J45" t="s">
         <v>398</v>
       </c>
-      <c r="J45" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3061,10 +3131,10 @@
         <v>399</v>
       </c>
       <c r="J46" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3090,13 +3160,13 @@
         <v>385</v>
       </c>
       <c r="I47" t="s">
+        <v>402</v>
+      </c>
+      <c r="J47" t="s">
         <v>398</v>
       </c>
-      <c r="J47" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3122,13 +3192,13 @@
         <v>385</v>
       </c>
       <c r="I48" t="s">
+        <v>401</v>
+      </c>
+      <c r="J48" t="s">
         <v>398</v>
       </c>
-      <c r="J48" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3157,10 +3227,10 @@
         <v>398</v>
       </c>
       <c r="J49" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3189,10 +3259,10 @@
         <v>398</v>
       </c>
       <c r="J50" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3221,10 +3291,10 @@
         <v>400</v>
       </c>
       <c r="J51" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3253,10 +3323,10 @@
         <v>400</v>
       </c>
       <c r="J52" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3285,10 +3355,10 @@
         <v>400</v>
       </c>
       <c r="J53" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3317,10 +3387,10 @@
         <v>400</v>
       </c>
       <c r="J54" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3346,13 +3416,13 @@
         <v>386</v>
       </c>
       <c r="I55" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J55" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3381,10 +3451,10 @@
         <v>398</v>
       </c>
       <c r="J56" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3410,13 +3480,13 @@
         <v>387</v>
       </c>
       <c r="I57" t="s">
+        <v>404</v>
+      </c>
+      <c r="J57" t="s">
         <v>398</v>
       </c>
-      <c r="J57" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3445,10 +3515,10 @@
         <v>400</v>
       </c>
       <c r="J58" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3477,10 +3547,10 @@
         <v>400</v>
       </c>
       <c r="J59" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3512,7 +3582,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3541,10 +3611,10 @@
         <v>400</v>
       </c>
       <c r="J61" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3573,10 +3643,10 @@
         <v>399</v>
       </c>
       <c r="J62" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3605,10 +3675,10 @@
         <v>402</v>
       </c>
       <c r="J63" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3637,10 +3707,10 @@
         <v>399</v>
       </c>
       <c r="J64" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3669,10 +3739,10 @@
         <v>400</v>
       </c>
       <c r="J65" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3704,7 +3774,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3733,10 +3803,10 @@
         <v>399</v>
       </c>
       <c r="J67" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3762,13 +3832,13 @@
         <v>388</v>
       </c>
       <c r="I68" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J68" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3794,13 +3864,13 @@
         <v>388</v>
       </c>
       <c r="I69" t="s">
+        <v>401</v>
+      </c>
+      <c r="J69" t="s">
         <v>399</v>
       </c>
-      <c r="J69" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3829,10 +3899,10 @@
         <v>399</v>
       </c>
       <c r="J70" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3861,10 +3931,10 @@
         <v>399</v>
       </c>
       <c r="J71" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3893,10 +3963,10 @@
         <v>399</v>
       </c>
       <c r="J72" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3925,10 +3995,10 @@
         <v>399</v>
       </c>
       <c r="J73" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3960,7 +4030,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3989,10 +4059,10 @@
         <v>399</v>
       </c>
       <c r="J75" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4024,7 +4094,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4053,10 +4123,10 @@
         <v>400</v>
       </c>
       <c r="J77" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4082,13 +4152,13 @@
         <v>389</v>
       </c>
       <c r="I78" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="J78" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4120,7 +4190,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4146,13 +4216,13 @@
         <v>389</v>
       </c>
       <c r="I80" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="J80" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4178,13 +4248,13 @@
         <v>389</v>
       </c>
       <c r="I81" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="J81" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4210,13 +4280,13 @@
         <v>390</v>
       </c>
       <c r="I82" t="s">
+        <v>404</v>
+      </c>
+      <c r="J82" t="s">
         <v>398</v>
       </c>
-      <c r="J82" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4242,13 +4312,13 @@
         <v>390</v>
       </c>
       <c r="I83" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J83" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4274,13 +4344,13 @@
         <v>390</v>
       </c>
       <c r="I84" t="s">
+        <v>401</v>
+      </c>
+      <c r="J84" t="s">
         <v>398</v>
       </c>
-      <c r="J84" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4309,10 +4379,10 @@
         <v>398</v>
       </c>
       <c r="J85" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4341,10 +4411,10 @@
         <v>399</v>
       </c>
       <c r="J86" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4370,13 +4440,13 @@
         <v>390</v>
       </c>
       <c r="I87" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J87" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4401,14 +4471,14 @@
       <c r="H88" t="s">
         <v>390</v>
       </c>
-      <c r="I88" t="s">
-        <v>405</v>
+      <c r="I88" s="2" t="s">
+        <v>403</v>
       </c>
       <c r="J88" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4434,13 +4504,13 @@
         <v>390</v>
       </c>
       <c r="I89" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="J89" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4466,13 +4536,13 @@
         <v>390</v>
       </c>
       <c r="I90" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="J90" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4497,14 +4567,14 @@
       <c r="H91" t="s">
         <v>390</v>
       </c>
-      <c r="I91" t="s">
+      <c r="I91" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="J91" t="s">
         <v>399</v>
       </c>
-      <c r="J91" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4530,13 +4600,13 @@
         <v>391</v>
       </c>
       <c r="I92" t="s">
+        <v>404</v>
+      </c>
+      <c r="J92" t="s">
         <v>398</v>
       </c>
-      <c r="J92" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -4565,10 +4635,10 @@
         <v>400</v>
       </c>
       <c r="J93" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4594,13 +4664,13 @@
         <v>391</v>
       </c>
       <c r="I94" t="s">
+        <v>401</v>
+      </c>
+      <c r="J94" t="s">
         <v>400</v>
       </c>
-      <c r="J94" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4626,13 +4696,13 @@
         <v>391</v>
       </c>
       <c r="I95" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J95" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4658,13 +4728,13 @@
         <v>391</v>
       </c>
       <c r="I96" t="s">
+        <v>400</v>
+      </c>
+      <c r="J96" t="s">
         <v>398</v>
       </c>
-      <c r="J96" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10">
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4693,10 +4763,10 @@
         <v>400</v>
       </c>
       <c r="J97" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4725,10 +4795,10 @@
         <v>400</v>
       </c>
       <c r="J98" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4754,13 +4824,13 @@
         <v>391</v>
       </c>
       <c r="I99" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J99" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4786,13 +4856,13 @@
         <v>391</v>
       </c>
       <c r="I100" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J100" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4821,10 +4891,10 @@
         <v>399</v>
       </c>
       <c r="J101" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4856,7 +4926,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -4885,10 +4955,10 @@
         <v>400</v>
       </c>
       <c r="J103" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -4917,10 +4987,10 @@
         <v>400</v>
       </c>
       <c r="J104" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -4949,10 +5019,10 @@
         <v>400</v>
       </c>
       <c r="J105" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -4981,10 +5051,10 @@
         <v>400</v>
       </c>
       <c r="J106" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -5013,10 +5083,10 @@
         <v>400</v>
       </c>
       <c r="J107" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -5045,10 +5115,10 @@
         <v>400</v>
       </c>
       <c r="J108" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -5077,10 +5147,10 @@
         <v>400</v>
       </c>
       <c r="J109" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -5112,7 +5182,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -5141,10 +5211,10 @@
         <v>400</v>
       </c>
       <c r="J111" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -5173,10 +5243,10 @@
         <v>400</v>
       </c>
       <c r="J112" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -5205,10 +5275,10 @@
         <v>400</v>
       </c>
       <c r="J113" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -5237,10 +5307,10 @@
         <v>400</v>
       </c>
       <c r="J114" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -5269,10 +5339,10 @@
         <v>400</v>
       </c>
       <c r="J115" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -5301,10 +5371,10 @@
         <v>400</v>
       </c>
       <c r="J116" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -5333,10 +5403,10 @@
         <v>400</v>
       </c>
       <c r="J117" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -5365,10 +5435,10 @@
         <v>400</v>
       </c>
       <c r="J118" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -5397,10 +5467,10 @@
         <v>400</v>
       </c>
       <c r="J119" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -5432,7 +5502,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -5461,10 +5531,10 @@
         <v>400</v>
       </c>
       <c r="J121" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -5496,7 +5566,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -5525,10 +5595,10 @@
         <v>400</v>
       </c>
       <c r="J123" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -5557,10 +5627,10 @@
         <v>400</v>
       </c>
       <c r="J124" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -5592,7 +5662,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -5621,10 +5691,10 @@
         <v>400</v>
       </c>
       <c r="J126" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -5653,10 +5723,10 @@
         <v>400</v>
       </c>
       <c r="J127" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -5685,10 +5755,10 @@
         <v>400</v>
       </c>
       <c r="J128" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -5717,10 +5787,10 @@
         <v>400</v>
       </c>
       <c r="J129" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -5749,10 +5819,10 @@
         <v>400</v>
       </c>
       <c r="J130" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -5781,10 +5851,10 @@
         <v>400</v>
       </c>
       <c r="J131" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -5816,7 +5886,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -5845,10 +5915,10 @@
         <v>400</v>
       </c>
       <c r="J133" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -5877,10 +5947,10 @@
         <v>400</v>
       </c>
       <c r="J134" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -5909,10 +5979,10 @@
         <v>400</v>
       </c>
       <c r="J135" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -5941,10 +6011,10 @@
         <v>400</v>
       </c>
       <c r="J136" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -5973,10 +6043,10 @@
         <v>400</v>
       </c>
       <c r="J137" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -6005,10 +6075,10 @@
         <v>400</v>
       </c>
       <c r="J138" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -6037,10 +6107,10 @@
         <v>400</v>
       </c>
       <c r="J139" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -6066,13 +6136,13 @@
         <v>396</v>
       </c>
       <c r="I140" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J140" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -6098,13 +6168,13 @@
         <v>396</v>
       </c>
       <c r="I141" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J141" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -6130,13 +6200,13 @@
         <v>396</v>
       </c>
       <c r="I142" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J142" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -6162,13 +6232,13 @@
         <v>396</v>
       </c>
       <c r="I143" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J143" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -6194,13 +6264,13 @@
         <v>396</v>
       </c>
       <c r="I144" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J144" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -6226,13 +6296,13 @@
         <v>396</v>
       </c>
       <c r="I145" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J145" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -6258,13 +6328,13 @@
         <v>396</v>
       </c>
       <c r="I146" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J146" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -6290,13 +6360,13 @@
         <v>396</v>
       </c>
       <c r="I147" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J147" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="148" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -6322,13 +6392,13 @@
         <v>396</v>
       </c>
       <c r="I148" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J148" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -6354,13 +6424,13 @@
         <v>396</v>
       </c>
       <c r="I149" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J149" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -6386,13 +6456,13 @@
         <v>396</v>
       </c>
       <c r="I150" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J150" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -6418,13 +6488,13 @@
         <v>396</v>
       </c>
       <c r="I151" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J151" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="152" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -6450,13 +6520,13 @@
         <v>397</v>
       </c>
       <c r="I152" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="J152" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="153" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -6482,13 +6552,13 @@
         <v>397</v>
       </c>
       <c r="I153" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="J153" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -6514,13 +6584,13 @@
         <v>397</v>
       </c>
       <c r="I154" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="J154" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -6546,13 +6616,13 @@
         <v>397</v>
       </c>
       <c r="I155" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="J155" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -6578,13 +6648,13 @@
         <v>397</v>
       </c>
       <c r="I156" t="s">
+        <v>404</v>
+      </c>
+      <c r="J156" t="s">
         <v>399</v>
       </c>
-      <c r="J156" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="157" spans="1:10">
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -6613,10 +6683,10 @@
         <v>404</v>
       </c>
       <c r="J157" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -6645,10 +6715,10 @@
         <v>404</v>
       </c>
       <c r="J158" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="159" spans="1:10">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -6677,10 +6747,10 @@
         <v>404</v>
       </c>
       <c r="J159" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -6706,13 +6776,13 @@
         <v>397</v>
       </c>
       <c r="I160" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="J160" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -6744,7 +6814,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -6773,10 +6843,10 @@
         <v>399</v>
       </c>
       <c r="J162" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="163" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -6808,7 +6878,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -6837,10 +6907,10 @@
         <v>399</v>
       </c>
       <c r="J164" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="165" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -6866,13 +6936,13 @@
         <v>397</v>
       </c>
       <c r="I165" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J165" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -6898,13 +6968,13 @@
         <v>397</v>
       </c>
       <c r="I166" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J166" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -6930,13 +7000,13 @@
         <v>397</v>
       </c>
       <c r="I167" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J167" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="168" spans="1:10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -6962,13 +7032,13 @@
         <v>397</v>
       </c>
       <c r="I168" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J168" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -6994,13 +7064,13 @@
         <v>397</v>
       </c>
       <c r="I169" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J169" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -7026,10 +7096,10 @@
         <v>397</v>
       </c>
       <c r="I170" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J170" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mapping of sdgs within pp bubbles and handling of pp columns in postprocessing
</commit_message>
<xml_diff>
--- a/postprocess/goal_target_list.xlsx
+++ b/postprocess/goal_target_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\SDG\Policy-Mapping\postprocess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4560E4D1-3234-4F61-89F8-9C9ED8FBCF02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031BCE69-520E-484D-BA9E-E7B5A49F7160}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="404">
   <si>
     <t>Target</t>
   </si>
@@ -1243,9 +1243,6 @@
   </si>
   <si>
     <t>Migration</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1656,14 +1653,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:L170"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="10" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -1719,9 +1713,6 @@
       <c r="H2" t="s">
         <v>381</v>
       </c>
-      <c r="I2" t="s">
-        <v>404</v>
-      </c>
       <c r="J2" t="s">
         <v>398</v>
       </c>
@@ -1751,9 +1742,6 @@
       <c r="H3" t="s">
         <v>381</v>
       </c>
-      <c r="I3" t="s">
-        <v>404</v>
-      </c>
       <c r="J3" t="s">
         <v>398</v>
       </c>
@@ -1786,9 +1774,6 @@
       <c r="I4" t="s">
         <v>398</v>
       </c>
-      <c r="J4" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1815,9 +1800,6 @@
       <c r="H5" t="s">
         <v>381</v>
       </c>
-      <c r="I5" t="s">
-        <v>404</v>
-      </c>
       <c r="J5" t="s">
         <v>398</v>
       </c>
@@ -1847,9 +1829,6 @@
       <c r="H6" t="s">
         <v>381</v>
       </c>
-      <c r="I6" t="s">
-        <v>404</v>
-      </c>
       <c r="J6" t="s">
         <v>398</v>
       </c>
@@ -1879,9 +1858,6 @@
       <c r="H7" t="s">
         <v>381</v>
       </c>
-      <c r="I7" t="s">
-        <v>404</v>
-      </c>
       <c r="J7" t="s">
         <v>398</v>
       </c>
@@ -1911,9 +1887,6 @@
       <c r="H8" t="s">
         <v>381</v>
       </c>
-      <c r="I8" t="s">
-        <v>404</v>
-      </c>
       <c r="J8" t="s">
         <v>398</v>
       </c>
@@ -1946,9 +1919,6 @@
       <c r="I9" t="s">
         <v>398</v>
       </c>
-      <c r="J9" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1978,9 +1948,6 @@
       <c r="I10" t="s">
         <v>398</v>
       </c>
-      <c r="J10" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -2010,9 +1977,6 @@
       <c r="I11" t="s">
         <v>399</v>
       </c>
-      <c r="J11" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -2074,9 +2038,6 @@
       <c r="I13" t="s">
         <v>400</v>
       </c>
-      <c r="J13" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -2135,9 +2096,6 @@
       <c r="H15" t="s">
         <v>382</v>
       </c>
-      <c r="I15" t="s">
-        <v>404</v>
-      </c>
       <c r="J15" t="s">
         <v>399</v>
       </c>
@@ -2170,9 +2128,6 @@
       <c r="I16" t="s">
         <v>399</v>
       </c>
-      <c r="J16" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -2202,9 +2157,6 @@
       <c r="I17" t="s">
         <v>398</v>
       </c>
-      <c r="J17" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -2234,9 +2186,6 @@
       <c r="I18" t="s">
         <v>398</v>
       </c>
-      <c r="J18" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -2266,9 +2215,6 @@
       <c r="I19" t="s">
         <v>398</v>
       </c>
-      <c r="J19" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -2295,9 +2241,6 @@
       <c r="H20" t="s">
         <v>383</v>
       </c>
-      <c r="I20" t="s">
-        <v>404</v>
-      </c>
       <c r="J20" t="s">
         <v>398</v>
       </c>
@@ -2327,9 +2270,6 @@
       <c r="H21" t="s">
         <v>383</v>
       </c>
-      <c r="I21" t="s">
-        <v>404</v>
-      </c>
       <c r="J21" t="s">
         <v>398</v>
       </c>
@@ -2359,9 +2299,6 @@
       <c r="H22" t="s">
         <v>383</v>
       </c>
-      <c r="I22" t="s">
-        <v>404</v>
-      </c>
       <c r="J22" t="s">
         <v>398</v>
       </c>
@@ -2394,9 +2331,6 @@
       <c r="I23" t="s">
         <v>398</v>
       </c>
-      <c r="J23" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -2426,9 +2360,6 @@
       <c r="I24" t="s">
         <v>398</v>
       </c>
-      <c r="J24" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -2487,9 +2418,6 @@
       <c r="H26" t="s">
         <v>383</v>
       </c>
-      <c r="I26" t="s">
-        <v>404</v>
-      </c>
       <c r="J26" t="s">
         <v>398</v>
       </c>
@@ -2522,9 +2450,6 @@
       <c r="I27" t="s">
         <v>398</v>
       </c>
-      <c r="J27" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -2554,9 +2479,6 @@
       <c r="I28" t="s">
         <v>398</v>
       </c>
-      <c r="J28" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -2586,9 +2508,6 @@
       <c r="I29" t="s">
         <v>398</v>
       </c>
-      <c r="J29" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -2618,9 +2537,6 @@
       <c r="I30" t="s">
         <v>398</v>
       </c>
-      <c r="J30" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -2650,9 +2566,6 @@
       <c r="I31" t="s">
         <v>398</v>
       </c>
-      <c r="J31" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -2679,9 +2592,6 @@
       <c r="H32" t="s">
         <v>384</v>
       </c>
-      <c r="I32" t="s">
-        <v>404</v>
-      </c>
       <c r="J32" t="s">
         <v>398</v>
       </c>
@@ -2807,9 +2717,6 @@
       <c r="H36" t="s">
         <v>384</v>
       </c>
-      <c r="I36" t="s">
-        <v>404</v>
-      </c>
       <c r="J36" t="s">
         <v>398</v>
       </c>
@@ -2906,9 +2813,6 @@
       <c r="I39" t="s">
         <v>398</v>
       </c>
-      <c r="J39" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
@@ -3031,9 +2935,6 @@
       <c r="H43" t="s">
         <v>385</v>
       </c>
-      <c r="I43" t="s">
-        <v>404</v>
-      </c>
       <c r="J43" t="s">
         <v>398</v>
       </c>
@@ -3095,9 +2996,6 @@
       <c r="H45" t="s">
         <v>385</v>
       </c>
-      <c r="I45" t="s">
-        <v>404</v>
-      </c>
       <c r="J45" t="s">
         <v>398</v>
       </c>
@@ -3226,9 +3124,6 @@
       <c r="I49" t="s">
         <v>398</v>
       </c>
-      <c r="J49" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
@@ -3258,9 +3153,6 @@
       <c r="I50" t="s">
         <v>398</v>
       </c>
-      <c r="J50" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
@@ -3290,9 +3182,6 @@
       <c r="I51" t="s">
         <v>400</v>
       </c>
-      <c r="J51" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
@@ -3322,9 +3211,6 @@
       <c r="I52" t="s">
         <v>400</v>
       </c>
-      <c r="J52" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
@@ -3386,9 +3272,6 @@
       <c r="I54" t="s">
         <v>400</v>
       </c>
-      <c r="J54" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
@@ -3418,9 +3301,6 @@
       <c r="I55" t="s">
         <v>400</v>
       </c>
-      <c r="J55" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
@@ -3479,9 +3359,6 @@
       <c r="H57" t="s">
         <v>387</v>
       </c>
-      <c r="I57" t="s">
-        <v>404</v>
-      </c>
       <c r="J57" t="s">
         <v>398</v>
       </c>
@@ -3514,9 +3391,6 @@
       <c r="I58" t="s">
         <v>400</v>
       </c>
-      <c r="J58" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
@@ -3578,9 +3452,6 @@
       <c r="I60" t="s">
         <v>400</v>
       </c>
-      <c r="J60" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
@@ -3610,9 +3481,6 @@
       <c r="I61" t="s">
         <v>400</v>
       </c>
-      <c r="J61" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
@@ -3642,9 +3510,6 @@
       <c r="I62" t="s">
         <v>399</v>
       </c>
-      <c r="J62" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
@@ -3706,9 +3571,6 @@
       <c r="I64" t="s">
         <v>399</v>
       </c>
-      <c r="J64" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
@@ -3738,9 +3600,6 @@
       <c r="I65" t="s">
         <v>400</v>
       </c>
-      <c r="J65" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
@@ -3802,9 +3661,6 @@
       <c r="I67" t="s">
         <v>399</v>
       </c>
-      <c r="J67" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
@@ -3898,9 +3754,6 @@
       <c r="I70" t="s">
         <v>399</v>
       </c>
-      <c r="J70" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
@@ -3962,9 +3815,6 @@
       <c r="I72" t="s">
         <v>399</v>
       </c>
-      <c r="J72" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
@@ -3994,9 +3844,6 @@
       <c r="I73" t="s">
         <v>399</v>
       </c>
-      <c r="J73" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
@@ -4026,9 +3873,6 @@
       <c r="I74" t="s">
         <v>399</v>
       </c>
-      <c r="J74" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
@@ -4058,9 +3902,6 @@
       <c r="I75" t="s">
         <v>399</v>
       </c>
-      <c r="J75" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
@@ -4090,9 +3931,6 @@
       <c r="I76" t="s">
         <v>399</v>
       </c>
-      <c r="J76" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
@@ -4186,9 +4024,6 @@
       <c r="I79" t="s">
         <v>399</v>
       </c>
-      <c r="J79" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
@@ -4279,9 +4114,6 @@
       <c r="H82" t="s">
         <v>390</v>
       </c>
-      <c r="I82" t="s">
-        <v>404</v>
-      </c>
       <c r="J82" t="s">
         <v>398</v>
       </c>
@@ -4410,9 +4242,6 @@
       <c r="I86" t="s">
         <v>399</v>
       </c>
-      <c r="J86" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
@@ -4442,9 +4271,6 @@
       <c r="I87" t="s">
         <v>401</v>
       </c>
-      <c r="J87" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
@@ -4474,9 +4300,6 @@
       <c r="I88" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="J88" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
@@ -4506,9 +4329,6 @@
       <c r="I89" t="s">
         <v>401</v>
       </c>
-      <c r="J89" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
@@ -4535,12 +4355,6 @@
       <c r="H90" t="s">
         <v>390</v>
       </c>
-      <c r="I90" t="s">
-        <v>404</v>
-      </c>
-      <c r="J90" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
@@ -4599,9 +4413,6 @@
       <c r="H92" t="s">
         <v>391</v>
       </c>
-      <c r="I92" t="s">
-        <v>404</v>
-      </c>
       <c r="J92" t="s">
         <v>398</v>
       </c>
@@ -4695,12 +4506,6 @@
       <c r="H95" t="s">
         <v>391</v>
       </c>
-      <c r="I95" t="s">
-        <v>404</v>
-      </c>
-      <c r="J95" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
@@ -4762,9 +4567,6 @@
       <c r="I97" t="s">
         <v>400</v>
       </c>
-      <c r="J97" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
@@ -4794,9 +4596,6 @@
       <c r="I98" t="s">
         <v>400</v>
       </c>
-      <c r="J98" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
@@ -4826,9 +4625,6 @@
       <c r="I99" t="s">
         <v>401</v>
       </c>
-      <c r="J99" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
@@ -4922,9 +4718,6 @@
       <c r="I102" t="s">
         <v>400</v>
       </c>
-      <c r="J102" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
@@ -4954,9 +4747,6 @@
       <c r="I103" t="s">
         <v>400</v>
       </c>
-      <c r="J103" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
@@ -4986,9 +4776,6 @@
       <c r="I104" t="s">
         <v>400</v>
       </c>
-      <c r="J104" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
@@ -5018,9 +4805,6 @@
       <c r="I105" t="s">
         <v>400</v>
       </c>
-      <c r="J105" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
@@ -5050,9 +4834,6 @@
       <c r="I106" t="s">
         <v>400</v>
       </c>
-      <c r="J106" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
@@ -5082,9 +4863,6 @@
       <c r="I107" t="s">
         <v>400</v>
       </c>
-      <c r="J107" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
@@ -5114,9 +4892,6 @@
       <c r="I108" t="s">
         <v>400</v>
       </c>
-      <c r="J108" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
@@ -5146,9 +4921,6 @@
       <c r="I109" t="s">
         <v>400</v>
       </c>
-      <c r="J109" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
@@ -5210,9 +4982,6 @@
       <c r="I111" t="s">
         <v>400</v>
       </c>
-      <c r="J111" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
@@ -5274,9 +5043,6 @@
       <c r="I113" t="s">
         <v>400</v>
       </c>
-      <c r="J113" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
@@ -5306,9 +5072,6 @@
       <c r="I114" t="s">
         <v>400</v>
       </c>
-      <c r="J114" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
@@ -5338,9 +5101,6 @@
       <c r="I115" t="s">
         <v>400</v>
       </c>
-      <c r="J115" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
@@ -5370,9 +5130,6 @@
       <c r="I116" t="s">
         <v>400</v>
       </c>
-      <c r="J116" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
@@ -5434,9 +5191,6 @@
       <c r="I118" t="s">
         <v>400</v>
       </c>
-      <c r="J118" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
@@ -5466,9 +5220,6 @@
       <c r="I119" t="s">
         <v>400</v>
       </c>
-      <c r="J119" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
@@ -5498,9 +5249,6 @@
       <c r="I120" t="s">
         <v>400</v>
       </c>
-      <c r="J120" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
@@ -5530,9 +5278,6 @@
       <c r="I121" t="s">
         <v>400</v>
       </c>
-      <c r="J121" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
@@ -5562,9 +5307,6 @@
       <c r="I122" t="s">
         <v>400</v>
       </c>
-      <c r="J122" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
@@ -5754,9 +5496,6 @@
       <c r="I128" t="s">
         <v>400</v>
       </c>
-      <c r="J128" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
@@ -5818,9 +5557,6 @@
       <c r="I130" t="s">
         <v>400</v>
       </c>
-      <c r="J130" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
@@ -5850,9 +5586,6 @@
       <c r="I131" t="s">
         <v>400</v>
       </c>
-      <c r="J131" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
@@ -5882,9 +5615,6 @@
       <c r="I132" t="s">
         <v>400</v>
       </c>
-      <c r="J132" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
@@ -5978,9 +5708,6 @@
       <c r="I135" t="s">
         <v>400</v>
       </c>
-      <c r="J135" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
@@ -6042,9 +5769,6 @@
       <c r="I137" t="s">
         <v>400</v>
       </c>
-      <c r="J137" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
@@ -6138,9 +5862,6 @@
       <c r="I140" t="s">
         <v>401</v>
       </c>
-      <c r="J140" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
@@ -6170,9 +5891,6 @@
       <c r="I141" t="s">
         <v>401</v>
       </c>
-      <c r="J141" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
@@ -6202,9 +5920,6 @@
       <c r="I142" t="s">
         <v>401</v>
       </c>
-      <c r="J142" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
@@ -6234,9 +5949,6 @@
       <c r="I143" t="s">
         <v>401</v>
       </c>
-      <c r="J143" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
@@ -6266,9 +5978,6 @@
       <c r="I144" t="s">
         <v>401</v>
       </c>
-      <c r="J144" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
@@ -6298,9 +6007,6 @@
       <c r="I145" t="s">
         <v>401</v>
       </c>
-      <c r="J145" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
@@ -6330,9 +6036,6 @@
       <c r="I146" t="s">
         <v>401</v>
       </c>
-      <c r="J146" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
@@ -6362,9 +6065,6 @@
       <c r="I147" t="s">
         <v>401</v>
       </c>
-      <c r="J147" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
@@ -6394,9 +6094,6 @@
       <c r="I148" t="s">
         <v>401</v>
       </c>
-      <c r="J148" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
@@ -6426,9 +6123,6 @@
       <c r="I149" t="s">
         <v>401</v>
       </c>
-      <c r="J149" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
@@ -6458,9 +6152,6 @@
       <c r="I150" t="s">
         <v>401</v>
       </c>
-      <c r="J150" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
@@ -6490,9 +6181,6 @@
       <c r="I151" t="s">
         <v>401</v>
       </c>
-      <c r="J151" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
@@ -6519,12 +6207,6 @@
       <c r="H152" t="s">
         <v>397</v>
       </c>
-      <c r="I152" t="s">
-        <v>404</v>
-      </c>
-      <c r="J152" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
@@ -6551,12 +6233,6 @@
       <c r="H153" t="s">
         <v>397</v>
       </c>
-      <c r="I153" t="s">
-        <v>404</v>
-      </c>
-      <c r="J153" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
@@ -6583,12 +6259,6 @@
       <c r="H154" t="s">
         <v>397</v>
       </c>
-      <c r="I154" t="s">
-        <v>404</v>
-      </c>
-      <c r="J154" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
@@ -6615,12 +6285,6 @@
       <c r="H155" t="s">
         <v>397</v>
       </c>
-      <c r="I155" t="s">
-        <v>404</v>
-      </c>
-      <c r="J155" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
@@ -6647,9 +6311,6 @@
       <c r="H156" t="s">
         <v>397</v>
       </c>
-      <c r="I156" t="s">
-        <v>404</v>
-      </c>
       <c r="J156" t="s">
         <v>399</v>
       </c>
@@ -6679,9 +6340,6 @@
       <c r="H157" t="s">
         <v>397</v>
       </c>
-      <c r="I157" t="s">
-        <v>404</v>
-      </c>
       <c r="J157" t="s">
         <v>402</v>
       </c>
@@ -6711,9 +6369,6 @@
       <c r="H158" t="s">
         <v>397</v>
       </c>
-      <c r="I158" t="s">
-        <v>404</v>
-      </c>
       <c r="J158" t="s">
         <v>402</v>
       </c>
@@ -6743,9 +6398,6 @@
       <c r="H159" t="s">
         <v>397</v>
       </c>
-      <c r="I159" t="s">
-        <v>404</v>
-      </c>
       <c r="J159" t="s">
         <v>402</v>
       </c>
@@ -6775,12 +6427,6 @@
       <c r="H160" t="s">
         <v>397</v>
       </c>
-      <c r="I160" t="s">
-        <v>404</v>
-      </c>
-      <c r="J160" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
@@ -6842,9 +6488,6 @@
       <c r="I162" t="s">
         <v>399</v>
       </c>
-      <c r="J162" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
@@ -6906,9 +6549,6 @@
       <c r="I164" t="s">
         <v>399</v>
       </c>
-      <c r="J164" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
@@ -6938,9 +6578,6 @@
       <c r="I165" t="s">
         <v>401</v>
       </c>
-      <c r="J165" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
@@ -6970,9 +6607,6 @@
       <c r="I166" t="s">
         <v>401</v>
       </c>
-      <c r="J166" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
@@ -6999,12 +6633,6 @@
       <c r="H167" t="s">
         <v>397</v>
       </c>
-      <c r="I167" t="s">
-        <v>404</v>
-      </c>
-      <c r="J167" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
@@ -7031,12 +6659,6 @@
       <c r="H168" t="s">
         <v>397</v>
       </c>
-      <c r="I168" t="s">
-        <v>404</v>
-      </c>
-      <c r="J168" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
@@ -7063,9 +6685,6 @@
       <c r="H169" t="s">
         <v>397</v>
       </c>
-      <c r="I169" t="s">
-        <v>404</v>
-      </c>
       <c r="J169" t="s">
         <v>401</v>
       </c>
@@ -7094,9 +6713,6 @@
       </c>
       <c r="H170" t="s">
         <v>397</v>
-      </c>
-      <c r="I170" t="s">
-        <v>404</v>
       </c>
       <c r="J170" t="s">
         <v>401</v>

</xml_diff>